<commit_message>
Site updated: 2020-12-04 22:40:24
</commit_message>
<xml_diff>
--- a/各端口服务漏洞/端口漏洞.xlsx
+++ b/各端口服务漏洞/端口漏洞.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hexo\source\_posts\各端口服务漏洞\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13C1FF1A-1B24-4026-A96C-9E905882619C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFDD170-8CA5-4ED3-8417-A4EEA1239089}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C8CC6791-FE15-4B8C-A8F2-6CCAFDA9AF5B}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C8CC6791-FE15-4B8C-A8F2-6CCAFDA9AF5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="162">
   <si>
     <t>Telnet远程访问</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -89,10 +83,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>爆破、Rlogin登录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Lotus domino邮件服务</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -208,10 +198,6 @@
   </si>
   <si>
     <t>RPC协议</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>域传送漏洞、劫持、缓存投毒、欺骗、CVE-2017-11779</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -511,12 +497,6 @@
   <si>
     <t>mqtt未授权访问
 nmap -p1883 --script=mqtt-subscribe IP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>未授权访问
-showmount、mount
-auxiliary/scanner/nfs/nfsmount</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -612,11 +592,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>auxiliary/scanner/x11/open_x11
-nmap -p6000 IP --script=x11-access</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>弱口令、爆破、未授权访问
 auxiliary/scanner/vnc/vnc_none_auth
 nmap -p5900 IP --script=vnc-brute</t>
@@ -656,11 +631,6 @@
   <si>
     <t>爆破
 nmap -p1080 IP --script=socks-brute</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>弱口令、爆破、搜集目标内网信息
-nmap -p161 IP --script=snmp-brute</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -727,6 +697,78 @@
   </si>
   <si>
     <t>QQ、socket</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>auxiliary/scanner/x11/open_x11
+unix/x11/x11_keyboard_exec
+nmap -p6000 IP --script=x11-access
+kali：xhost +
+xwd -screen -root -silent -display IP:0 &gt; screenshot.xwd
+convert screenshot.xwd screenshot.png</t>
+  </si>
+  <si>
+    <t>2375、2376</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未授权访问
+curl -s http://IP:2376/version | python -m json.tool
+docker -H &lt;host&gt;:&lt;port&gt; info
+docker -H &lt;host&gt;:&lt;port&gt; ps
+docker -H &lt;host&gt;:&lt;port&gt; images
+docker -H &lt;host&gt;:&lt;port&gt; exec -it &lt;container name&gt; /bin/bash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>curl -v -X POST 'http://ip:8088/ws/v1/cluster/apps/new-application'</t>
+  </si>
+  <si>
+    <t>弱口令、爆破、搜集目标内网信息
+弱口令检测：nmap –sU –p161 –script=snmp-brute 目标ip //查找snmp弱口令
+弱口令利用：nmap -sU -p161 --script=snmp-netstat 目标ip//获取网络端口状态
+nmap –sU –p161 –script=snmp-sysdescr 目标ip //获取系统信息
+nmap -sU -p161 --script=snmp-win32-user 目标ip //获取用户信息
+snmputil walk ip public .1.3.6.1.2.1.25.4.2.1.2//列出系统进程
+snmputil walk ip public.1.3.6.1.2.1.25.6.3.1.2 //列出安装的软件
+snmputil walk ip public .1.3.6.1.2.1.1 //列出系统信息
+snmputil get  ip public .1.3.6.1.4.1.77.1.4.1.0 //列出域名
+snmputil walk ip public.1.3.6.1.4.1.77.1.2.25.1.1 //列系统用户列表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爆破、Rlogin登录
+rlogin IP
+rlogin IP -l [username] //指定用户名登录
+chkconfig --list //检测rlogin服务是否开启
+chkconfig rlogin on //开启rlogin服务</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>域传送漏洞、劫持、缓存投毒、欺骗、CVE-2017-11779
+nmap --script dns-zone-transfer --script-args dns-zone-trans
+fer.domain=[domain/ip] -p 53 -Pn dns.domain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>未授权访问
+rpcinfo -p IP //检测是否启用NFS服务
+showmount -e IP //列出可导出的目录列表
+showmount IP //连接的主机
+showmount -d IP //目录
+showmount -a IP //挂载点
+mount -t nfs IP:/ /tmp //指定IP的根目录挂载到/tmp目录下
+MSF：auxiliary/scanner/nfs/nfsmount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nexus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CVE-2020-10199：Nexus Repository Manager OSS/PRo &lt;=3.21.1，需有低权限账号。
+CVE-2020-10204：Nexus Repository Manager OSS/PRo &lt;=3.21.1，需有管理员账号。
+默认账号密码：admin/admin123</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1160,42 +1202,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B4E82-55DE-4071-8DEE-B5CCE8EF821E}">
-  <dimension ref="B2:D67"/>
+  <dimension ref="B2:D69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.796875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="19.296875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="49.69921875" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.59765625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.19921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="62.19921875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="20.25" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="131.25" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B4" s="5">
         <v>22</v>
       </c>
@@ -1203,7 +1245,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
@@ -1214,21 +1256,21 @@
         <v>0</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="112.5" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>53</v>
       </c>
@@ -1236,12 +1278,12 @@
         <v>2</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>3</v>
@@ -1255,32 +1297,32 @@
         <v>69</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
@@ -1288,10 +1330,10 @@
         <v>111</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -1299,12 +1341,12 @@
         <v>135</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
@@ -1315,27 +1357,27 @@
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="262.5" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="150" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="131.25" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>389</v>
       </c>
@@ -1343,7 +1385,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
@@ -1351,10 +1393,10 @@
         <v>443</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="75" x14ac:dyDescent="0.25">
@@ -1365,10 +1407,10 @@
         <v>11</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="93.75" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>12</v>
       </c>
@@ -1376,7 +1418,7 @@
         <v>13</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>14</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="112.5" x14ac:dyDescent="0.25">
@@ -1384,10 +1426,10 @@
         <v>873</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
@@ -1395,21 +1437,21 @@
         <v>1080</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
@@ -1417,32 +1459,32 @@
         <v>1352</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="6" t="s">
+    </row>
+    <row r="26" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="B26" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="B26" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="D26" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
@@ -1450,21 +1492,21 @@
         <v>1883</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="150" x14ac:dyDescent="0.25">
       <c r="B28" s="5">
         <v>2049</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>118</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
@@ -1472,21 +1514,21 @@
         <v>2181</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="5">
-        <v>2375</v>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="B30" s="5" t="s">
+        <v>153</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
@@ -1494,10 +1536,10 @@
         <v>2601</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
@@ -1505,21 +1547,21 @@
         <v>3128</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="93.75" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B33" s="5">
         <v>3306</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
@@ -1527,10 +1569,10 @@
         <v>3389</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
@@ -1538,10 +1580,10 @@
         <v>3690</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
@@ -1549,10 +1591,10 @@
         <v>4440</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
@@ -1560,10 +1602,10 @@
         <v>4560</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
@@ -1571,21 +1613,21 @@
         <v>4750</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -1593,21 +1635,21 @@
         <v>4899</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="42" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
@@ -1615,43 +1657,43 @@
         <v>5432</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B43" s="5" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
       <c r="B44" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="112.5" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
@@ -1659,32 +1701,32 @@
         <v>6379</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="D48" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
@@ -1692,213 +1734,235 @@
         <v>8069</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" ht="93.75" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D50" s="6" t="s">
         <v>97</v>
-      </c>
-      <c r="D50" s="6" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="51" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" ht="93.75" x14ac:dyDescent="0.25">
+      <c r="B52" s="5">
+        <v>8081</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B54" s="5">
+        <v>8088</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B55" s="5">
+        <v>8161</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="5">
+        <v>9000</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="5">
+        <v>9001</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D51" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B53" s="5">
-        <v>8161</v>
-      </c>
-      <c r="C53" s="1" t="s">
+      <c r="D57" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="D53" s="6" t="s">
+    </row>
+    <row r="58" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B58" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" ht="262.5" x14ac:dyDescent="0.25">
+      <c r="B59" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="5">
+        <v>10000</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B61" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="B62" s="5">
+        <v>11211</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B63" s="5">
+        <v>12345</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" s="5">
-        <v>9000</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D54" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="5">
-        <v>9001</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D55" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B56" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" ht="300" x14ac:dyDescent="0.25">
-      <c r="B57" s="5" t="s">
+      <c r="D63" s="6" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B64" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" s="5">
-        <v>10000</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B59" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C59" s="1" t="s">
+      <c r="C64" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D59" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="B60" s="5">
-        <v>11211</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D60" s="6" t="s">
+      <c r="D64" s="6" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="5">
-        <v>12345</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D61" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="62" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B62" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D62" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="63" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B63" s="5">
-        <v>50000</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="64" spans="2:4" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="B64" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="65" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B65" s="5">
-        <v>60020</v>
+        <v>50000</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="66" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="B66" s="5">
-        <v>60030</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B66" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>85</v>
+        <v>122</v>
       </c>
     </row>
     <row r="67" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="B67" s="5">
-        <v>61616</v>
+        <v>60020</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>80</v>
       </c>
       <c r="D67" s="6" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B68" s="5">
+        <v>60030</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="69" spans="2:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="B69" s="5">
+        <v>61616</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>